<commit_message>
Regenerated IG's after minor fixes - markdown file fixes, ImplementationGuide fixes, etc.
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/practitionerrole-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/practitionerrole-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$100</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3500" uniqueCount="417">
   <si>
     <t>Path</t>
   </si>
@@ -955,6 +955,126 @@
     <t>https://healthterminologies.gov.au/fhir/ValueSet/anzsco-1</t>
   </si>
   <si>
+    <t>PractitionerRole.code.coding.id</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.extension</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.system</t>
+  </si>
+  <si>
+    <t>Identity of the terminology system</t>
+  </si>
+  <si>
+    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
+  </si>
+  <si>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should de-reference to some definition that establish the system clearly and unambiguously.</t>
+  </si>
+  <si>
+    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>http://www.abs.gov.au/ausstats/abs@.nsf/mf/1220.0</t>
+  </si>
+  <si>
+    <t>Coding.system</t>
+  </si>
+  <si>
+    <t>C*E.3</t>
+  </si>
+  <si>
+    <t>./codeSystem</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.version</t>
+  </si>
+  <si>
+    <t>Version of the system - if relevant</t>
+  </si>
+  <si>
+    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured. and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
+  </si>
+  <si>
+    <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
+  </si>
+  <si>
+    <t>Coding.version</t>
+  </si>
+  <si>
+    <t>C*E.7</t>
+  </si>
+  <si>
+    <t>./codeSystemVersion</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.code</t>
+  </si>
+  <si>
+    <t>Symbol in syntax defined by the system</t>
+  </si>
+  <si>
+    <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
+  </si>
+  <si>
+    <t>Need to refer to a particular code in the system.</t>
+  </si>
+  <si>
+    <t>Coding.code</t>
+  </si>
+  <si>
+    <t>C*E.1</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.display</t>
+  </si>
+  <si>
+    <t>Representation defined by the system</t>
+  </si>
+  <si>
+    <t>A representation of the meaning of the code in the system, following the rules of the system.</t>
+  </si>
+  <si>
+    <t>Need to be able to carry a human-readable meaning of the code for readers that do not know  the system.</t>
+  </si>
+  <si>
+    <t>Coding.display</t>
+  </si>
+  <si>
+    <t>C*E.2 - but note this is not well followed</t>
+  </si>
+  <si>
+    <t>CV.displayName</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.userSelected</t>
+  </si>
+  <si>
+    <t>If this coding was chosen directly by the user</t>
+  </si>
+  <si>
+    <t>Indicates that this coding was chosen by a user directly - i.e. off a pick list of available items (codes or displays).</t>
+  </si>
+  <si>
+    <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
+  </si>
+  <si>
+    <t>This has been identified as a clinical safety criterium - that this exact system/code pair was chosen explicitly, rather than inferred by the system based on some rules or language processing.</t>
+  </si>
+  <si>
+    <t>Coding.userSelected</t>
+  </si>
+  <si>
+    <t>Sometimes implied by being first</t>
+  </si>
+  <si>
+    <t>CD.codingRationale</t>
+  </si>
+  <si>
     <t>SNOMEDPractitionerRoleCode</t>
   </si>
   <si>
@@ -962,6 +1082,9 @@
   </si>
   <si>
     <t>https://healthterminologies.gov.au/fhir/ValueSet/practitioner-role-1</t>
+  </si>
+  <si>
+    <t>http://snomed.info/sct</t>
   </si>
   <si>
     <t>PractitionerRole.code.text</t>
@@ -1348,7 +1471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM86"/>
+  <dimension ref="A1:AM100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -8518,11 +8641,9 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="B65" t="s" s="2">
         <v>297</v>
       </c>
+      <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8540,23 +8661,19 @@
         <v>40</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>298</v>
+        <v>122</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>159</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8580,13 +8697,13 @@
         <v>40</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>299</v>
+        <v>40</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>40</v>
@@ -8604,13 +8721,13 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>40</v>
@@ -8619,10 +8736,10 @@
         <v>40</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
@@ -8633,18 +8750,18 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>40</v>
@@ -8653,23 +8770,21 @@
         <v>40</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>228</v>
+        <v>127</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>167</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>40</v>
       </c>
@@ -8705,25 +8820,25 @@
         <v>40</v>
       </c>
       <c r="AA66" t="s" s="2">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="AB66" t="s" s="2">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="AC66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD66" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>40</v>
@@ -8732,10 +8847,10 @@
         <v>40</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
@@ -8744,9 +8859,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8754,13 +8869,13 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>40</v>
@@ -8769,22 +8884,26 @@
         <v>52</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="L67" t="s" s="2">
+      <c r="N67" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" t="s" s="2">
-        <v>40</v>
+        <v>304</v>
       </c>
       <c r="R67" t="s" s="2">
         <v>40</v>
@@ -8802,11 +8921,13 @@
         <v>40</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="X67" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y67" t="s" s="2">
-        <v>299</v>
+        <v>40</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>40</v>
@@ -8824,13 +8945,13 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>40</v>
@@ -8839,19 +8960,19 @@
         <v>40</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
         <v>308</v>
       </c>
@@ -8864,10 +8985,10 @@
         <v>41</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H68" t="s" s="2">
         <v>40</v>
@@ -8876,15 +8997,17 @@
         <v>52</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L68" t="s" s="2">
+      <c r="M68" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
         <v>40</v>
@@ -8933,13 +9056,13 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>40</v>
@@ -8948,19 +9071,19 @@
         <v>40</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>40</v>
+        <v>313</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>313</v>
+        <v>40</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>314</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
         <v>315</v>
       </c>
@@ -8973,28 +9096,30 @@
         <v>41</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I69" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H69" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J69" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K69" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="K69" t="s" s="2">
+      <c r="L69" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" s="2"/>
+      <c r="N69" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>40</v>
       </c>
@@ -9042,13 +9167,13 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>40</v>
@@ -9057,10 +9182,10 @@
         <v>40</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
@@ -9069,9 +9194,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9082,10 +9207,10 @@
         <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H70" t="s" s="2">
         <v>40</v>
@@ -9094,7 +9219,7 @@
         <v>52</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>322</v>
+        <v>121</v>
       </c>
       <c r="K70" t="s" s="2">
         <v>323</v>
@@ -9153,13 +9278,13 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>40</v>
@@ -9168,10 +9293,10 @@
         <v>40</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>40</v>
+        <v>327</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>40</v>
@@ -9180,9 +9305,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9193,30 +9318,32 @@
         <v>41</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I71" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J71" t="s" s="2">
-        <v>328</v>
+        <v>253</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N71" s="2"/>
+        <v>332</v>
+      </c>
+      <c r="N71" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="O71" t="s" s="2">
         <v>40</v>
       </c>
@@ -9264,25 +9391,25 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH71" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>332</v>
+        <v>40</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>40</v>
+        <v>335</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>40</v>
@@ -9293,9 +9420,11 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="B72" s="2"/>
+        <v>292</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>337</v>
+      </c>
       <c r="C72" t="s" s="2">
         <v>40</v>
       </c>
@@ -9313,19 +9442,23 @@
         <v>40</v>
       </c>
       <c r="I72" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>122</v>
+        <v>338</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
+        <v>282</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>159</v>
+      </c>
       <c r="O72" t="s" s="2">
         <v>40</v>
       </c>
@@ -9349,13 +9482,13 @@
         <v>40</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>40</v>
+        <v>339</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>40</v>
@@ -9373,13 +9506,13 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>40</v>
@@ -9388,10 +9521,10 @@
         <v>40</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>40</v>
@@ -9402,18 +9535,18 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>40</v>
@@ -9425,17 +9558,15 @@
         <v>40</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
         <v>40</v>
@@ -9484,13 +9615,13 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>40</v>
@@ -9513,11 +9644,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>337</v>
+        <v>96</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9530,19 +9661,19 @@
         <v>40</v>
       </c>
       <c r="H74" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
         <v>97</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>338</v>
+        <v>127</v>
       </c>
       <c r="M74" t="s" s="2">
         <v>100</v>
@@ -9583,19 +9714,19 @@
         <v>40</v>
       </c>
       <c r="AA74" t="s" s="2">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="AC74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD74" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>339</v>
+        <v>130</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9613,7 +9744,7 @@
         <v>40</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
@@ -9622,9 +9753,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>340</v>
+        <v>299</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9632,37 +9763,41 @@
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I75" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J75" t="s" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>341</v>
+        <v>300</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="M75" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N75" t="s" s="2">
+        <v>303</v>
+      </c>
       <c r="O75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P75" s="2"/>
       <c r="Q75" t="s" s="2">
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="R75" t="s" s="2">
         <v>40</v>
@@ -9680,13 +9815,13 @@
         <v>40</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>343</v>
+        <v>40</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>344</v>
+        <v>40</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>40</v>
@@ -9704,13 +9839,13 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>40</v>
@@ -9719,10 +9854,10 @@
         <v>40</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
@@ -9731,9 +9866,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>345</v>
+        <v>308</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9747,24 +9882,26 @@
         <v>51</v>
       </c>
       <c r="G76" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H76" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I76" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J76" t="s" s="2">
-        <v>253</v>
+        <v>121</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>346</v>
+        <v>309</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="M76" s="2"/>
+        <v>310</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>311</v>
+      </c>
       <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>40</v>
@@ -9813,7 +9950,7 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>345</v>
+        <v>312</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -9828,10 +9965,10 @@
         <v>40</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>40</v>
+        <v>313</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
@@ -9840,9 +9977,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>348</v>
+        <v>315</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9856,27 +9993,27 @@
         <v>51</v>
       </c>
       <c r="G77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I77" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J77" t="s" s="2">
-        <v>349</v>
+        <v>70</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N77" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="M77" s="2"/>
+      <c r="N77" t="s" s="2">
+        <v>318</v>
+      </c>
       <c r="O77" t="s" s="2">
         <v>40</v>
       </c>
@@ -9924,7 +10061,7 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -9939,10 +10076,10 @@
         <v>40</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>40</v>
+        <v>320</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
@@ -9951,9 +10088,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>353</v>
+        <v>322</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9967,27 +10104,27 @@
         <v>51</v>
       </c>
       <c r="G78" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H78" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I78" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J78" t="s" s="2">
-        <v>349</v>
+        <v>121</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N78" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="M78" s="2"/>
+      <c r="N78" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="O78" t="s" s="2">
         <v>40</v>
       </c>
@@ -10035,7 +10172,7 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -10050,10 +10187,10 @@
         <v>40</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>40</v>
+        <v>327</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>40</v>
@@ -10062,9 +10199,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10075,28 +10212,32 @@
         <v>41</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G79" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H79" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I79" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I79" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J79" t="s" s="2">
-        <v>328</v>
+        <v>253</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
+        <v>331</v>
+      </c>
+      <c r="M79" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="N79" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="O79" t="s" s="2">
         <v>40</v>
       </c>
@@ -10144,25 +10285,25 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG79" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH79" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>332</v>
+        <v>40</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>40</v>
+        <v>335</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>40</v>
@@ -10173,7 +10314,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10193,19 +10334,23 @@
         <v>40</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J80" t="s" s="2">
         <v>121</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="M80" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N80" t="s" s="2">
+        <v>167</v>
+      </c>
       <c r="O80" t="s" s="2">
         <v>40</v>
       </c>
@@ -10253,7 +10398,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10268,10 +10413,10 @@
         <v>40</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>40</v>
@@ -10280,13 +10425,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" hidden="true">
+    <row r="81">
       <c r="A81" t="s" s="2">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" t="s" s="2">
@@ -10296,26 +10441,24 @@
         <v>42</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I81" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>98</v>
+        <v>343</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" t="s" s="2">
         <v>40</v>
@@ -10340,13 +10483,11 @@
         <v>40</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="X81" s="2"/>
       <c r="Y81" t="s" s="2">
-        <v>40</v>
+        <v>339</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>40</v>
@@ -10364,7 +10505,7 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>130</v>
+        <v>342</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -10379,25 +10520,25 @@
         <v>40</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>40</v>
+        <v>346</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>125</v>
+        <v>347</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>40</v>
+        <v>348</v>
       </c>
       <c r="AM81" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="82" hidden="true">
+    <row r="82">
       <c r="A82" t="s" s="2">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>337</v>
+        <v>40</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -10407,26 +10548,24 @@
         <v>42</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H82" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I82" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>97</v>
+        <v>350</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>103</v>
+        <v>351</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
         <v>40</v>
@@ -10475,7 +10614,7 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10493,18 +10632,18 @@
         <v>40</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>94</v>
+        <v>353</v>
       </c>
       <c r="AL82" t="s" s="2">
-        <v>40</v>
+        <v>354</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>40</v>
+        <v>355</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10512,10 +10651,10 @@
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>52</v>
@@ -10527,13 +10666,13 @@
         <v>40</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>121</v>
+        <v>357</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -10584,13 +10723,13 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>40</v>
@@ -10599,10 +10738,10 @@
         <v>40</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>125</v>
+        <v>361</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>40</v>
@@ -10613,7 +10752,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10624,7 +10763,7 @@
         <v>41</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>52</v>
@@ -10633,19 +10772,21 @@
         <v>40</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>192</v>
+        <v>363</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L84" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="M84" s="2"/>
+      <c r="N84" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="L84" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
         <v>40</v>
       </c>
@@ -10693,13 +10834,13 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG84" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH84" t="s" s="2">
         <v>40</v>
@@ -10711,7 +10852,7 @@
         <v>40</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>333</v>
+        <v>367</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>40</v>
@@ -10733,7 +10874,7 @@
         <v>41</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>52</v>
@@ -10745,15 +10886,17 @@
         <v>40</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>121</v>
+        <v>369</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M85" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>372</v>
+      </c>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
         <v>40</v>
@@ -10808,19 +10951,19 @@
         <v>41</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>40</v>
+        <v>373</v>
       </c>
       <c r="AJ85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>333</v>
+        <v>374</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>40</v>
@@ -10831,7 +10974,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10842,7 +10985,7 @@
         <v>41</v>
       </c>
       <c r="F86" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G86" t="s" s="2">
         <v>40</v>
@@ -10854,18 +10997,16 @@
         <v>40</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>372</v>
+        <v>121</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>373</v>
+        <v>122</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>374</v>
+        <v>123</v>
       </c>
       <c r="M86" s="2"/>
-      <c r="N86" t="s" s="2">
-        <v>375</v>
-      </c>
+      <c r="N86" s="2"/>
       <c r="O86" t="s" s="2">
         <v>40</v>
       </c>
@@ -10913,13 +11054,13 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>371</v>
+        <v>124</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG86" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH86" t="s" s="2">
         <v>40</v>
@@ -10940,8 +11081,1548 @@
         <v>40</v>
       </c>
     </row>
+    <row r="87" hidden="true">
+      <c r="A87" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F87" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J87" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M87" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N87" s="2"/>
+      <c r="O87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P87" s="2"/>
+      <c r="Q87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM87" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" hidden="true">
+      <c r="A88" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F88" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N88" s="2"/>
+      <c r="O88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM88" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F89" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G89" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P89" s="2"/>
+      <c r="Q89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM89" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F90" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G90" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J90" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="K90" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P90" s="2"/>
+      <c r="Q90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE90" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AF90" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG90" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM90" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G91" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="N91" s="2"/>
+      <c r="O91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P91" s="2"/>
+      <c r="Q91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM91" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F92" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G92" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M92" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="N92" s="2"/>
+      <c r="O92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM92" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F93" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM93" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F94" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P94" s="2"/>
+      <c r="Q94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM94" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F95" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N95" s="2"/>
+      <c r="O95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P95" s="2"/>
+      <c r="Q95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F96" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N96" s="2"/>
+      <c r="O96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P96" s="2"/>
+      <c r="Q96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM96" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P97" s="2"/>
+      <c r="Q97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM97" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F98" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G98" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J98" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L98" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P98" s="2"/>
+      <c r="Q98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM98" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F99" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G99" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J99" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K99" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="L99" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+      <c r="O99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P99" s="2"/>
+      <c r="Q99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE99" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="AF99" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG99" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK99" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM99" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" hidden="true">
+      <c r="A100" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F100" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J100" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="K100" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L100" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M100" s="2"/>
+      <c r="N100" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P100" s="2"/>
+      <c r="Q100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE100" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="AF100" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG100" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK100" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM100" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AM86">
+  <autoFilter ref="A1:AM100">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10951,7 +12632,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI85">
+  <conditionalFormatting sqref="A2:AI99">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerated ACR,ES,PHR,PDL,SHS,SML Ig's after many narrative bugfixes and improvements to profiles.
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/practitionerrole-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/practitionerrole-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$100</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3500" uniqueCount="417">
   <si>
     <t>Path</t>
   </si>
@@ -955,6 +955,126 @@
     <t>https://healthterminologies.gov.au/fhir/ValueSet/anzsco-1</t>
   </si>
   <si>
+    <t>PractitionerRole.code.coding.id</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.extension</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.system</t>
+  </si>
+  <si>
+    <t>Identity of the terminology system</t>
+  </si>
+  <si>
+    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
+  </si>
+  <si>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should de-reference to some definition that establish the system clearly and unambiguously.</t>
+  </si>
+  <si>
+    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>http://www.abs.gov.au/ausstats/abs@.nsf/mf/1220.0</t>
+  </si>
+  <si>
+    <t>Coding.system</t>
+  </si>
+  <si>
+    <t>C*E.3</t>
+  </si>
+  <si>
+    <t>./codeSystem</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.version</t>
+  </si>
+  <si>
+    <t>Version of the system - if relevant</t>
+  </si>
+  <si>
+    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured. and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
+  </si>
+  <si>
+    <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
+  </si>
+  <si>
+    <t>Coding.version</t>
+  </si>
+  <si>
+    <t>C*E.7</t>
+  </si>
+  <si>
+    <t>./codeSystemVersion</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.code</t>
+  </si>
+  <si>
+    <t>Symbol in syntax defined by the system</t>
+  </si>
+  <si>
+    <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
+  </si>
+  <si>
+    <t>Need to refer to a particular code in the system.</t>
+  </si>
+  <si>
+    <t>Coding.code</t>
+  </si>
+  <si>
+    <t>C*E.1</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.display</t>
+  </si>
+  <si>
+    <t>Representation defined by the system</t>
+  </si>
+  <si>
+    <t>A representation of the meaning of the code in the system, following the rules of the system.</t>
+  </si>
+  <si>
+    <t>Need to be able to carry a human-readable meaning of the code for readers that do not know  the system.</t>
+  </si>
+  <si>
+    <t>Coding.display</t>
+  </si>
+  <si>
+    <t>C*E.2 - but note this is not well followed</t>
+  </si>
+  <si>
+    <t>CV.displayName</t>
+  </si>
+  <si>
+    <t>PractitionerRole.code.coding.userSelected</t>
+  </si>
+  <si>
+    <t>If this coding was chosen directly by the user</t>
+  </si>
+  <si>
+    <t>Indicates that this coding was chosen by a user directly - i.e. off a pick list of available items (codes or displays).</t>
+  </si>
+  <si>
+    <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
+  </si>
+  <si>
+    <t>This has been identified as a clinical safety criterium - that this exact system/code pair was chosen explicitly, rather than inferred by the system based on some rules or language processing.</t>
+  </si>
+  <si>
+    <t>Coding.userSelected</t>
+  </si>
+  <si>
+    <t>Sometimes implied by being first</t>
+  </si>
+  <si>
+    <t>CD.codingRationale</t>
+  </si>
+  <si>
     <t>SNOMEDPractitionerRoleCode</t>
   </si>
   <si>
@@ -962,6 +1082,9 @@
   </si>
   <si>
     <t>https://healthterminologies.gov.au/fhir/ValueSet/practitioner-role-1</t>
+  </si>
+  <si>
+    <t>http://snomed.info/sct</t>
   </si>
   <si>
     <t>PractitionerRole.code.text</t>
@@ -1348,7 +1471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM86"/>
+  <dimension ref="A1:AM100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -8518,11 +8641,9 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="B65" t="s" s="2">
         <v>297</v>
       </c>
+      <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8540,23 +8661,19 @@
         <v>40</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>298</v>
+        <v>122</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>159</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8580,13 +8697,13 @@
         <v>40</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>299</v>
+        <v>40</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>40</v>
@@ -8604,13 +8721,13 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>40</v>
@@ -8619,10 +8736,10 @@
         <v>40</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
@@ -8633,18 +8750,18 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>40</v>
@@ -8653,23 +8770,21 @@
         <v>40</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>228</v>
+        <v>127</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>167</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>40</v>
       </c>
@@ -8705,25 +8820,25 @@
         <v>40</v>
       </c>
       <c r="AA66" t="s" s="2">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="AB66" t="s" s="2">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="AC66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD66" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>40</v>
@@ -8732,10 +8847,10 @@
         <v>40</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
@@ -8744,9 +8859,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8754,13 +8869,13 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>40</v>
@@ -8769,22 +8884,26 @@
         <v>52</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="L67" t="s" s="2">
+      <c r="N67" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" t="s" s="2">
-        <v>40</v>
+        <v>304</v>
       </c>
       <c r="R67" t="s" s="2">
         <v>40</v>
@@ -8802,11 +8921,13 @@
         <v>40</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="X67" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y67" t="s" s="2">
-        <v>299</v>
+        <v>40</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>40</v>
@@ -8824,13 +8945,13 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>40</v>
@@ -8839,19 +8960,19 @@
         <v>40</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
         <v>308</v>
       </c>
@@ -8864,10 +8985,10 @@
         <v>41</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H68" t="s" s="2">
         <v>40</v>
@@ -8876,15 +8997,17 @@
         <v>52</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L68" t="s" s="2">
+      <c r="M68" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
         <v>40</v>
@@ -8933,13 +9056,13 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>40</v>
@@ -8948,19 +9071,19 @@
         <v>40</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>40</v>
+        <v>313</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>313</v>
+        <v>40</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>314</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
         <v>315</v>
       </c>
@@ -8973,28 +9096,30 @@
         <v>41</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I69" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H69" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J69" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K69" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="K69" t="s" s="2">
+      <c r="L69" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" s="2"/>
+      <c r="N69" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>40</v>
       </c>
@@ -9042,13 +9167,13 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>40</v>
@@ -9057,10 +9182,10 @@
         <v>40</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
@@ -9069,9 +9194,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9082,10 +9207,10 @@
         <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H70" t="s" s="2">
         <v>40</v>
@@ -9094,7 +9219,7 @@
         <v>52</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>322</v>
+        <v>121</v>
       </c>
       <c r="K70" t="s" s="2">
         <v>323</v>
@@ -9153,13 +9278,13 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>40</v>
@@ -9168,10 +9293,10 @@
         <v>40</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>40</v>
+        <v>327</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>40</v>
@@ -9180,9 +9305,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9193,30 +9318,32 @@
         <v>41</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I71" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J71" t="s" s="2">
-        <v>328</v>
+        <v>253</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N71" s="2"/>
+        <v>332</v>
+      </c>
+      <c r="N71" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="O71" t="s" s="2">
         <v>40</v>
       </c>
@@ -9264,25 +9391,25 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH71" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>332</v>
+        <v>40</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>40</v>
+        <v>335</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>40</v>
@@ -9293,9 +9420,11 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="B72" s="2"/>
+        <v>292</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>337</v>
+      </c>
       <c r="C72" t="s" s="2">
         <v>40</v>
       </c>
@@ -9313,19 +9442,23 @@
         <v>40</v>
       </c>
       <c r="I72" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>122</v>
+        <v>338</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
+        <v>282</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>159</v>
+      </c>
       <c r="O72" t="s" s="2">
         <v>40</v>
       </c>
@@ -9349,13 +9482,13 @@
         <v>40</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>40</v>
+        <v>339</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>40</v>
@@ -9373,13 +9506,13 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>40</v>
@@ -9388,10 +9521,10 @@
         <v>40</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>40</v>
@@ -9402,18 +9535,18 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>40</v>
@@ -9425,17 +9558,15 @@
         <v>40</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
         <v>40</v>
@@ -9484,13 +9615,13 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>40</v>
@@ -9513,11 +9644,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>337</v>
+        <v>96</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9530,19 +9661,19 @@
         <v>40</v>
       </c>
       <c r="H74" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
         <v>97</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>338</v>
+        <v>127</v>
       </c>
       <c r="M74" t="s" s="2">
         <v>100</v>
@@ -9583,19 +9714,19 @@
         <v>40</v>
       </c>
       <c r="AA74" t="s" s="2">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="AC74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD74" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>339</v>
+        <v>130</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9613,7 +9744,7 @@
         <v>40</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
@@ -9622,9 +9753,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>340</v>
+        <v>299</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9632,37 +9763,41 @@
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I75" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J75" t="s" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>341</v>
+        <v>300</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="M75" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N75" t="s" s="2">
+        <v>303</v>
+      </c>
       <c r="O75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P75" s="2"/>
       <c r="Q75" t="s" s="2">
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="R75" t="s" s="2">
         <v>40</v>
@@ -9680,13 +9815,13 @@
         <v>40</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>343</v>
+        <v>40</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>344</v>
+        <v>40</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>40</v>
@@ -9704,13 +9839,13 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>40</v>
@@ -9719,10 +9854,10 @@
         <v>40</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
@@ -9731,9 +9866,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>345</v>
+        <v>308</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9747,24 +9882,26 @@
         <v>51</v>
       </c>
       <c r="G76" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H76" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I76" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J76" t="s" s="2">
-        <v>253</v>
+        <v>121</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>346</v>
+        <v>309</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="M76" s="2"/>
+        <v>310</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>311</v>
+      </c>
       <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>40</v>
@@ -9813,7 +9950,7 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>345</v>
+        <v>312</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -9828,10 +9965,10 @@
         <v>40</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>40</v>
+        <v>313</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
@@ -9840,9 +9977,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>348</v>
+        <v>315</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9856,27 +9993,27 @@
         <v>51</v>
       </c>
       <c r="G77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I77" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J77" t="s" s="2">
-        <v>349</v>
+        <v>70</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N77" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="M77" s="2"/>
+      <c r="N77" t="s" s="2">
+        <v>318</v>
+      </c>
       <c r="O77" t="s" s="2">
         <v>40</v>
       </c>
@@ -9924,7 +10061,7 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -9939,10 +10076,10 @@
         <v>40</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>40</v>
+        <v>320</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
@@ -9951,9 +10088,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>353</v>
+        <v>322</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9967,27 +10104,27 @@
         <v>51</v>
       </c>
       <c r="G78" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H78" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I78" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J78" t="s" s="2">
-        <v>349</v>
+        <v>121</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N78" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="M78" s="2"/>
+      <c r="N78" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="O78" t="s" s="2">
         <v>40</v>
       </c>
@@ -10035,7 +10172,7 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -10050,10 +10187,10 @@
         <v>40</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>40</v>
+        <v>327</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>40</v>
@@ -10062,9 +10199,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10075,28 +10212,32 @@
         <v>41</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G79" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H79" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I79" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I79" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J79" t="s" s="2">
-        <v>328</v>
+        <v>253</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
+        <v>331</v>
+      </c>
+      <c r="M79" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="N79" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="O79" t="s" s="2">
         <v>40</v>
       </c>
@@ -10144,25 +10285,25 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG79" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH79" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>332</v>
+        <v>40</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>40</v>
+        <v>335</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>40</v>
@@ -10173,7 +10314,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10193,19 +10334,23 @@
         <v>40</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J80" t="s" s="2">
         <v>121</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="M80" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N80" t="s" s="2">
+        <v>167</v>
+      </c>
       <c r="O80" t="s" s="2">
         <v>40</v>
       </c>
@@ -10253,7 +10398,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10268,10 +10413,10 @@
         <v>40</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>40</v>
@@ -10280,13 +10425,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" hidden="true">
+    <row r="81">
       <c r="A81" t="s" s="2">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" t="s" s="2">
@@ -10296,26 +10441,24 @@
         <v>42</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I81" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>98</v>
+        <v>343</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" t="s" s="2">
         <v>40</v>
@@ -10340,13 +10483,11 @@
         <v>40</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="X81" s="2"/>
       <c r="Y81" t="s" s="2">
-        <v>40</v>
+        <v>339</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>40</v>
@@ -10364,7 +10505,7 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>130</v>
+        <v>342</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -10379,25 +10520,25 @@
         <v>40</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>40</v>
+        <v>346</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>125</v>
+        <v>347</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>40</v>
+        <v>348</v>
       </c>
       <c r="AM81" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="82" hidden="true">
+    <row r="82">
       <c r="A82" t="s" s="2">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>337</v>
+        <v>40</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -10407,26 +10548,24 @@
         <v>42</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H82" t="s" s="2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I82" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>97</v>
+        <v>350</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>103</v>
+        <v>351</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
         <v>40</v>
@@ -10475,7 +10614,7 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10493,18 +10632,18 @@
         <v>40</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>94</v>
+        <v>353</v>
       </c>
       <c r="AL82" t="s" s="2">
-        <v>40</v>
+        <v>354</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>40</v>
+        <v>355</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10512,10 +10651,10 @@
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>52</v>
@@ -10527,13 +10666,13 @@
         <v>40</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>121</v>
+        <v>357</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -10584,13 +10723,13 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>40</v>
@@ -10599,10 +10738,10 @@
         <v>40</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>125</v>
+        <v>361</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>40</v>
@@ -10613,7 +10752,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10624,7 +10763,7 @@
         <v>41</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>52</v>
@@ -10633,19 +10772,21 @@
         <v>40</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>192</v>
+        <v>363</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L84" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="M84" s="2"/>
+      <c r="N84" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="L84" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
         <v>40</v>
       </c>
@@ -10693,13 +10834,13 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG84" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH84" t="s" s="2">
         <v>40</v>
@@ -10711,7 +10852,7 @@
         <v>40</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>333</v>
+        <v>367</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>40</v>
@@ -10733,7 +10874,7 @@
         <v>41</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>52</v>
@@ -10745,15 +10886,17 @@
         <v>40</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>121</v>
+        <v>369</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M85" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>372</v>
+      </c>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
         <v>40</v>
@@ -10808,19 +10951,19 @@
         <v>41</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AH85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>40</v>
+        <v>373</v>
       </c>
       <c r="AJ85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>333</v>
+        <v>374</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>40</v>
@@ -10831,7 +10974,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10842,7 +10985,7 @@
         <v>41</v>
       </c>
       <c r="F86" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G86" t="s" s="2">
         <v>40</v>
@@ -10854,18 +10997,16 @@
         <v>40</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>372</v>
+        <v>121</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>373</v>
+        <v>122</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>374</v>
+        <v>123</v>
       </c>
       <c r="M86" s="2"/>
-      <c r="N86" t="s" s="2">
-        <v>375</v>
-      </c>
+      <c r="N86" s="2"/>
       <c r="O86" t="s" s="2">
         <v>40</v>
       </c>
@@ -10913,13 +11054,13 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>371</v>
+        <v>124</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG86" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AH86" t="s" s="2">
         <v>40</v>
@@ -10940,8 +11081,1548 @@
         <v>40</v>
       </c>
     </row>
+    <row r="87" hidden="true">
+      <c r="A87" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F87" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J87" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M87" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N87" s="2"/>
+      <c r="O87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P87" s="2"/>
+      <c r="Q87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM87" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" hidden="true">
+      <c r="A88" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F88" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N88" s="2"/>
+      <c r="O88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM88" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F89" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G89" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P89" s="2"/>
+      <c r="Q89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM89" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F90" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G90" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J90" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="K90" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P90" s="2"/>
+      <c r="Q90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE90" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AF90" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG90" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM90" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G91" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="N91" s="2"/>
+      <c r="O91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P91" s="2"/>
+      <c r="Q91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM91" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F92" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G92" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M92" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="N92" s="2"/>
+      <c r="O92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM92" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F93" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM93" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F94" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P94" s="2"/>
+      <c r="Q94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM94" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F95" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N95" s="2"/>
+      <c r="O95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P95" s="2"/>
+      <c r="Q95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F96" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N96" s="2"/>
+      <c r="O96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P96" s="2"/>
+      <c r="Q96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM96" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P97" s="2"/>
+      <c r="Q97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM97" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F98" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G98" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J98" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L98" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P98" s="2"/>
+      <c r="Q98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM98" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F99" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G99" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J99" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="K99" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="L99" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+      <c r="O99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P99" s="2"/>
+      <c r="Q99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE99" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="AF99" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG99" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK99" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM99" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" hidden="true">
+      <c r="A100" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F100" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J100" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="K100" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L100" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M100" s="2"/>
+      <c r="N100" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P100" s="2"/>
+      <c r="Q100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE100" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="AF100" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG100" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK100" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AL100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM100" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AM86">
+  <autoFilter ref="A1:AM100">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10951,7 +12632,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI85">
+  <conditionalFormatting sqref="A2:AI99">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>